<commit_message>
Updated app.py with transparent overlay fix
</commit_message>
<xml_diff>
--- a/S3- MicroNet Template.xlsx
+++ b/S3- MicroNet Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccireland-my.sharepoint.com/personal/nsoledadrioscolombo_ucc_ie/Documents/Natalia Rios/Experiments/SIHUMI Network Model/SIHUMI/Open_Source_Version/Python_ver/MNP_Merge_Dummy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My_Git_Projects\micronet_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{4ED1C126-E095-4B7D-87BF-6789476A9FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1116C05-D3D6-4354-92F7-1CC4F39D0EA2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C150ED2-A1C8-48F2-B7A6-0F347C3BEBF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Positive" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
   <si>
     <t>B. longum</t>
   </si>
@@ -61,27 +61,9 @@
     <t>E. faecalis</t>
   </si>
   <si>
-    <t>nodeFontSize</t>
-  </si>
-  <si>
     <t>scale neutral strength</t>
   </si>
   <si>
-    <t>scale linewidth</t>
-  </si>
-  <si>
-    <t>scale arrowsize</t>
-  </si>
-  <si>
-    <t>combined transparency</t>
-  </si>
-  <si>
-    <t>nodeSize</t>
-  </si>
-  <si>
-    <t>nodeColor</t>
-  </si>
-  <si>
     <t>Positive Line Color</t>
   </si>
   <si>
@@ -110,6 +92,21 @@
   </si>
   <si>
     <t>#D88A4B</t>
+  </si>
+  <si>
+    <t>Linewidth</t>
+  </si>
+  <si>
+    <t>Arrowsize</t>
+  </si>
+  <si>
+    <t>FontSize</t>
+  </si>
+  <si>
+    <t>NodeSize</t>
+  </si>
+  <si>
+    <t>NodeColor</t>
   </si>
 </sst>
 </file>
@@ -220,10 +217,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1010,11 +1003,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E30C8B70-53F8-4C31-B528-9EE08736CD68}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
@@ -1024,7 +1015,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2">
         <v>1.5</v>
@@ -1032,7 +1023,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2">
         <v>12</v>
@@ -1040,83 +1031,79 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="14.25" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2">
-        <v>16</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2">
-        <v>200</v>
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
         <v>15</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
+        <v>12</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2"/>
@@ -1128,29 +1115,25 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="B19" s="4"/>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="B16" s="2"/>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="4"/>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="2:2">
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="2:2">
       <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="B24" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>